<commit_message>
Update Modelo Planilha de Locacao.xlsx
</commit_message>
<xml_diff>
--- a/Modelo Planilha de Locacao.xlsx
+++ b/Modelo Planilha de Locacao.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msj\Documents\GitHub\pyToScriptCAD\in\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3AAC4D8-7E3F-4BCF-94D0-6384C023DD37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01B1300E-BF45-44C1-90CB-C2AA7A988405}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-45" windowWidth="29040" windowHeight="15720" tabRatio="831" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Lista" sheetId="87" r:id="rId1"/>
+    <sheet name="Locacao" sheetId="87" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <t>A</t>
   </si>
@@ -71,9 +71,6 @@
   </si>
   <si>
     <t>Programado</t>
-  </si>
-  <si>
-    <t>Layers</t>
   </si>
   <si>
     <t>Cancelado</t>
@@ -178,7 +175,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -242,42 +239,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -313,23 +279,14 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="4" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="2" fontId="1" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -347,10 +304,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -650,9 +603,9 @@
   <sheetFormatPr defaultColWidth="3.88671875" defaultRowHeight="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.44140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="7.109375" style="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7" style="20" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.6640625" style="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="7.109375" style="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7" style="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" style="18" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.88671875" style="5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="2.77734375" style="3" customWidth="1"/>
     <col min="8" max="8" width="15" style="6" bestFit="1" customWidth="1"/>
@@ -686,17 +639,23 @@
         <v>7</v>
       </c>
       <c r="G1" s="8"/>
-      <c r="H1" s="17" t="s">
+      <c r="H1" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="18"/>
+      <c r="I1" s="20"/>
       <c r="J1" s="8"/>
-      <c r="K1" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="L1" s="22"/>
-      <c r="M1" s="22"/>
-      <c r="N1" s="23"/>
+      <c r="K1" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="M1" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1" s="9" t="s">
+        <v>23</v>
+      </c>
       <c r="O1" s="8"/>
     </row>
     <row r="2" spans="1:15" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -724,18 +683,14 @@
         <v>1</v>
       </c>
       <c r="J2" s="2"/>
-      <c r="K2" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="L2" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="M2" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="N2" s="9" t="s">
-        <v>24</v>
-      </c>
+      <c r="K2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
       <c r="O2" s="2"/>
     </row>
     <row r="3" spans="1:15" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -755,18 +710,18 @@
         <v>12</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I3" s="4">
         <v>1</v>
       </c>
       <c r="J3" s="2"/>
       <c r="K3" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="L3" s="4" t="s">
         <v>18</v>
@@ -789,19 +744,19 @@
         <v>5.68</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F4" s="13"/>
       <c r="G4" s="2"/>
       <c r="H4" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I4" s="4">
         <v>0.5</v>
       </c>
       <c r="J4" s="2"/>
       <c r="K4" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="L4" s="4" t="s">
         <v>19</v>
@@ -821,12 +776,8 @@
       <c r="H5" s="9"/>
       <c r="I5" s="4"/>
       <c r="J5" s="2"/>
-      <c r="K5" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="L5" s="4" t="s">
-        <v>20</v>
-      </c>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
       <c r="M5" s="4"/>
       <c r="N5" s="4"/>
       <c r="O5" s="2"/>
@@ -918,10 +869,10 @@
     </row>
     <row r="11" spans="1:15" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="14"/>
-      <c r="B11" s="19"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="19"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
       <c r="F11" s="12"/>
       <c r="G11" s="2"/>
       <c r="H11" s="9"/>
@@ -935,10 +886,10 @@
     </row>
     <row r="12" spans="1:15" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="14"/>
-      <c r="B12" s="19"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
       <c r="F12" s="10"/>
       <c r="G12" s="2"/>
       <c r="H12" s="9"/>
@@ -3790,9 +3741,8 @@
       <c r="O179" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="1">
     <mergeCell ref="H1:I1"/>
-    <mergeCell ref="K1:N1"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>